<commit_message>
Remove old code and run reports again.
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -824,7 +824,7 @@
         <v>6</v>
       </c>
       <c r="Y3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -937,9 +937,6 @@
       <c r="P6">
         <v>3</v>
       </c>
-      <c r="Q6">
-        <v>12</v>
-      </c>
       <c r="R6">
         <v>6</v>
       </c>
@@ -2446,6 +2443,12 @@
         <v>102</v>
       </c>
       <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>12</v>
+      </c>
+      <c r="Y43">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix output files NA string
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="148">
   <si>
     <t>Cell_Type</t>
   </si>
@@ -322,7 +322,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>&lt;NA&gt;</t>
+    <t>NA</t>
   </si>
   <si>
     <t>45</t>
@@ -356,9 +356,6 @@
   </si>
   <si>
     <t>47</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Severe</t>
@@ -924,7 +921,7 @@
         <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
         <v>102</v>
@@ -945,7 +942,7 @@
         <v>102</v>
       </c>
       <c r="N2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O2" t="s">
         <v>102</v>
@@ -954,7 +951,7 @@
         <v>102</v>
       </c>
       <c r="Q2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R2" t="s">
         <v>102</v>
@@ -981,7 +978,7 @@
         <v>102</v>
       </c>
       <c r="Z2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AA2" t="s">
         <v>102</v>
@@ -1004,7 +1001,7 @@
         <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H3" t="s">
         <v>102</v>
@@ -1031,7 +1028,7 @@
         <v>102</v>
       </c>
       <c r="P3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q3" t="s">
         <v>102</v>
@@ -1058,7 +1055,7 @@
         <v>102</v>
       </c>
       <c r="Y3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z3" t="s">
         <v>102</v>
@@ -1087,34 +1084,34 @@
         <v>129.4299011230469</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N4" t="s">
         <v>102</v>
       </c>
       <c r="O4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q4" t="s">
         <v>102</v>
@@ -1123,7 +1120,7 @@
         <v>102</v>
       </c>
       <c r="S4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T4" t="s">
         <v>102</v>
@@ -1132,7 +1129,7 @@
         <v>102</v>
       </c>
       <c r="V4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W4" t="s">
         <v>102</v>
@@ -1141,13 +1138,13 @@
         <v>102</v>
       </c>
       <c r="Y4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z4" t="s">
         <v>102</v>
       </c>
       <c r="AA4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -1167,7 +1164,7 @@
         <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
         <v>102</v>
@@ -1247,7 +1244,7 @@
         <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
         <v>102</v>
@@ -1256,16 +1253,16 @@
         <v>104</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N6" t="s">
         <v>102</v>
@@ -1274,19 +1271,19 @@
         <v>102</v>
       </c>
       <c r="P6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q6" t="s">
         <v>102</v>
       </c>
       <c r="R6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U6" t="s">
         <v>102</v>
@@ -1298,10 +1295,10 @@
         <v>102</v>
       </c>
       <c r="X6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Y6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Z6" t="s">
         <v>102</v>
@@ -1327,67 +1324,67 @@
         <v>102</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
         <v>102</v>
       </c>
       <c r="I7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K7" t="s">
+        <v>133</v>
+      </c>
+      <c r="L7" t="s">
+        <v>142</v>
+      </c>
+      <c r="M7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N7" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P7" t="s">
         <v>132</v>
       </c>
-      <c r="J7" t="s">
+      <c r="Q7" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" t="s">
         <v>134</v>
       </c>
-      <c r="K7" t="s">
-        <v>134</v>
-      </c>
-      <c r="L7" t="s">
-        <v>143</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="T7" t="s">
+        <v>145</v>
+      </c>
+      <c r="U7" t="s">
+        <v>102</v>
+      </c>
+      <c r="V7" t="s">
+        <v>145</v>
+      </c>
+      <c r="W7" t="s">
+        <v>102</v>
+      </c>
+      <c r="X7" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y7" t="s">
         <v>132</v>
       </c>
-      <c r="N7" t="s">
-        <v>102</v>
-      </c>
-      <c r="O7" t="s">
-        <v>124</v>
-      </c>
-      <c r="P7" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>102</v>
-      </c>
-      <c r="R7" t="s">
-        <v>146</v>
-      </c>
-      <c r="S7" t="s">
-        <v>135</v>
-      </c>
-      <c r="T7" t="s">
-        <v>146</v>
-      </c>
-      <c r="U7" t="s">
-        <v>102</v>
-      </c>
-      <c r="V7" t="s">
-        <v>146</v>
-      </c>
-      <c r="W7" t="s">
-        <v>102</v>
-      </c>
-      <c r="X7" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>133</v>
-      </c>
       <c r="Z7" t="s">
         <v>102</v>
       </c>
       <c r="AA7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1410,7 +1407,7 @@
         <v>118.6440963745117</v>
       </c>
       <c r="G8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
         <v>102</v>
@@ -1437,7 +1434,7 @@
         <v>102</v>
       </c>
       <c r="P8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q8" t="s">
         <v>102</v>
@@ -1464,7 +1461,7 @@
         <v>102</v>
       </c>
       <c r="Y8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z8" t="s">
         <v>102</v>
@@ -1493,34 +1490,34 @@
         <v>140.5238952636719</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
         <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K9" t="s">
+        <v>146</v>
+      </c>
+      <c r="L9" t="s">
+        <v>137</v>
+      </c>
+      <c r="M9" t="s">
+        <v>137</v>
+      </c>
+      <c r="N9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9" t="s">
         <v>147</v>
       </c>
-      <c r="L9" t="s">
-        <v>138</v>
-      </c>
-      <c r="M9" t="s">
-        <v>138</v>
-      </c>
-      <c r="N9" t="s">
-        <v>102</v>
-      </c>
-      <c r="O9" t="s">
-        <v>148</v>
-      </c>
       <c r="P9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q9" t="s">
         <v>102</v>
@@ -1535,10 +1532,10 @@
         <v>102</v>
       </c>
       <c r="U9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W9" t="s">
         <v>102</v>
@@ -1547,13 +1544,13 @@
         <v>102</v>
       </c>
       <c r="Y9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z9" t="s">
         <v>102</v>
       </c>
       <c r="AA9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1576,7 +1573,7 @@
         <v>110.0154037475586</v>
       </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
         <v>102</v>
@@ -1600,10 +1597,10 @@
         <v>102</v>
       </c>
       <c r="O10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q10" t="s">
         <v>102</v>
@@ -1618,7 +1615,7 @@
         <v>102</v>
       </c>
       <c r="U10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V10" t="s">
         <v>102</v>
@@ -1630,13 +1627,13 @@
         <v>102</v>
       </c>
       <c r="Y10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z10" t="s">
         <v>102</v>
       </c>
       <c r="AA10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1659,7 +1656,7 @@
         <v>130.66259765625</v>
       </c>
       <c r="G11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
         <v>102</v>
@@ -1686,13 +1683,13 @@
         <v>102</v>
       </c>
       <c r="P11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q11" t="s">
         <v>102</v>
       </c>
       <c r="R11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S11" t="s">
         <v>102</v>
@@ -1713,7 +1710,7 @@
         <v>102</v>
       </c>
       <c r="Y11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z11" t="s">
         <v>102</v>
@@ -1742,7 +1739,7 @@
         <v>100.1540985107422</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s">
         <v>102</v>
@@ -1751,58 +1748,58 @@
         <v>102</v>
       </c>
       <c r="J12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N12" t="s">
+        <v>137</v>
+      </c>
+      <c r="O12" t="s">
         <v>138</v>
       </c>
-      <c r="O12" t="s">
-        <v>139</v>
-      </c>
       <c r="P12" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>102</v>
+      </c>
+      <c r="R12" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" t="s">
+        <v>102</v>
+      </c>
+      <c r="T12" t="s">
+        <v>145</v>
+      </c>
+      <c r="U12" t="s">
+        <v>102</v>
+      </c>
+      <c r="V12" t="s">
+        <v>102</v>
+      </c>
+      <c r="W12" t="s">
+        <v>102</v>
+      </c>
+      <c r="X12" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA12" t="s">
         <v>138</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>102</v>
-      </c>
-      <c r="R12" t="s">
-        <v>102</v>
-      </c>
-      <c r="S12" t="s">
-        <v>102</v>
-      </c>
-      <c r="T12" t="s">
-        <v>146</v>
-      </c>
-      <c r="U12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V12" t="s">
-        <v>102</v>
-      </c>
-      <c r="W12" t="s">
-        <v>102</v>
-      </c>
-      <c r="X12" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>138</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1825,10 +1822,10 @@
         <v>129.4299011230469</v>
       </c>
       <c r="G13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I13" t="s">
         <v>102</v>
@@ -1849,10 +1846,10 @@
         <v>102</v>
       </c>
       <c r="O13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q13" t="s">
         <v>102</v>
@@ -1873,19 +1870,19 @@
         <v>102</v>
       </c>
       <c r="W13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="X13" t="s">
         <v>102</v>
       </c>
       <c r="Y13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z13" t="s">
         <v>102</v>
       </c>
       <c r="AA13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1908,25 +1905,25 @@
         <v>125.8860015869141</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H14" t="s">
         <v>102</v>
       </c>
       <c r="I14" t="s">
+        <v>133</v>
+      </c>
+      <c r="J14" t="s">
+        <v>137</v>
+      </c>
+      <c r="K14" t="s">
         <v>134</v>
       </c>
-      <c r="J14" t="s">
-        <v>138</v>
-      </c>
-      <c r="K14" t="s">
-        <v>135</v>
-      </c>
       <c r="L14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N14" t="s">
         <v>102</v>
@@ -1935,13 +1932,13 @@
         <v>102</v>
       </c>
       <c r="P14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q14" t="s">
         <v>102</v>
       </c>
       <c r="R14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S14" t="s">
         <v>102</v>
@@ -1962,7 +1959,7 @@
         <v>102</v>
       </c>
       <c r="Y14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z14" t="s">
         <v>102</v>
@@ -1991,26 +1988,26 @@
         <v>131.7411041259766</v>
       </c>
       <c r="G15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H15" t="s">
         <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K15" t="s">
+        <v>145</v>
+      </c>
+      <c r="L15" t="s">
+        <v>147</v>
+      </c>
+      <c r="M15" t="s">
         <v>146</v>
       </c>
-      <c r="L15" t="s">
-        <v>148</v>
-      </c>
-      <c r="M15" t="s">
-        <v>147</v>
-      </c>
       <c r="N15" t="s">
         <v>102</v>
       </c>
@@ -2018,7 +2015,7 @@
         <v>102</v>
       </c>
       <c r="P15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q15" t="s">
         <v>102</v>
@@ -2033,7 +2030,7 @@
         <v>102</v>
       </c>
       <c r="U15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V15" t="s">
         <v>102</v>
@@ -2045,7 +2042,7 @@
         <v>102</v>
       </c>
       <c r="Y15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z15" t="s">
         <v>102</v>
@@ -2074,34 +2071,34 @@
         <v>114.021598815918</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I16" t="s">
         <v>102</v>
       </c>
       <c r="J16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N16" t="s">
         <v>102</v>
       </c>
       <c r="O16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q16" t="s">
         <v>102</v>
@@ -2110,7 +2107,7 @@
         <v>102</v>
       </c>
       <c r="S16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T16" t="s">
         <v>102</v>
@@ -2125,16 +2122,16 @@
         <v>102</v>
       </c>
       <c r="X16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z16" t="s">
         <v>102</v>
       </c>
       <c r="AA16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -2157,34 +2154,34 @@
         <v>69.33744049072266</v>
       </c>
       <c r="G17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N17" t="s">
         <v>102</v>
       </c>
       <c r="O17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q17" t="s">
         <v>102</v>
@@ -2193,7 +2190,7 @@
         <v>102</v>
       </c>
       <c r="S17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T17" t="s">
         <v>102</v>
@@ -2202,7 +2199,7 @@
         <v>102</v>
       </c>
       <c r="V17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W17" t="s">
         <v>102</v>
@@ -2211,13 +2208,13 @@
         <v>102</v>
       </c>
       <c r="Y17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z17" t="s">
         <v>102</v>
       </c>
       <c r="AA17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -2240,7 +2237,7 @@
         <v>114.6379013061523</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
         <v>102</v>
@@ -2264,10 +2261,10 @@
         <v>102</v>
       </c>
       <c r="O18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q18" t="s">
         <v>102</v>
@@ -2291,16 +2288,16 @@
         <v>102</v>
       </c>
       <c r="X18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z18" t="s">
         <v>102</v>
       </c>
       <c r="AA18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -2323,13 +2320,13 @@
         <v>76.27118682861328</v>
       </c>
       <c r="G19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J19" t="s">
         <v>102</v>
@@ -2347,10 +2344,10 @@
         <v>102</v>
       </c>
       <c r="O19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q19" t="s">
         <v>102</v>
@@ -2362,13 +2359,13 @@
         <v>102</v>
       </c>
       <c r="T19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U19" t="s">
         <v>102</v>
       </c>
       <c r="V19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W19" t="s">
         <v>102</v>
@@ -2377,13 +2374,13 @@
         <v>102</v>
       </c>
       <c r="Y19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z19" t="s">
         <v>102</v>
       </c>
       <c r="AA19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2406,7 +2403,7 @@
         <v>111.2481002807617</v>
       </c>
       <c r="G20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" t="s">
         <v>102</v>
@@ -2415,16 +2412,16 @@
         <v>102</v>
       </c>
       <c r="J20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N20" t="s">
         <v>102</v>
@@ -2433,7 +2430,7 @@
         <v>102</v>
       </c>
       <c r="P20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q20" t="s">
         <v>102</v>
@@ -2445,7 +2442,7 @@
         <v>102</v>
       </c>
       <c r="T20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U20" t="s">
         <v>102</v>
@@ -2460,7 +2457,7 @@
         <v>102</v>
       </c>
       <c r="Y20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z20" t="s">
         <v>102</v>
@@ -2489,67 +2486,67 @@
         <v>110.9399032592773</v>
       </c>
       <c r="G21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J21" t="s">
+        <v>145</v>
+      </c>
+      <c r="K21" t="s">
+        <v>145</v>
+      </c>
+      <c r="L21" t="s">
         <v>146</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
+        <v>145</v>
+      </c>
+      <c r="N21" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>102</v>
+      </c>
+      <c r="R21" t="s">
+        <v>102</v>
+      </c>
+      <c r="S21" t="s">
         <v>146</v>
       </c>
-      <c r="L21" t="s">
+      <c r="T21" t="s">
+        <v>102</v>
+      </c>
+      <c r="U21" t="s">
+        <v>102</v>
+      </c>
+      <c r="V21" t="s">
+        <v>102</v>
+      </c>
+      <c r="W21" t="s">
+        <v>102</v>
+      </c>
+      <c r="X21" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA21" t="s">
         <v>147</v>
-      </c>
-      <c r="M21" t="s">
-        <v>146</v>
-      </c>
-      <c r="N21" t="s">
-        <v>102</v>
-      </c>
-      <c r="O21" t="s">
-        <v>148</v>
-      </c>
-      <c r="P21" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>102</v>
-      </c>
-      <c r="R21" t="s">
-        <v>102</v>
-      </c>
-      <c r="S21" t="s">
-        <v>147</v>
-      </c>
-      <c r="T21" t="s">
-        <v>102</v>
-      </c>
-      <c r="U21" t="s">
-        <v>102</v>
-      </c>
-      <c r="V21" t="s">
-        <v>102</v>
-      </c>
-      <c r="W21" t="s">
-        <v>102</v>
-      </c>
-      <c r="X21" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -2572,25 +2569,25 @@
         <v>74.57627105712891</v>
       </c>
       <c r="G22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N22" t="s">
         <v>102</v>
@@ -2599,16 +2596,16 @@
         <v>102</v>
       </c>
       <c r="P22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q22" t="s">
         <v>102</v>
       </c>
       <c r="R22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T22" t="s">
         <v>102</v>
@@ -2626,7 +2623,7 @@
         <v>102</v>
       </c>
       <c r="Y22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z22" t="s">
         <v>102</v>
@@ -2655,25 +2652,25 @@
         <v>84.12943267822266</v>
       </c>
       <c r="G23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" t="s">
         <v>117</v>
       </c>
-      <c r="H23" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" t="s">
-        <v>118</v>
-      </c>
       <c r="J23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N23" t="s">
         <v>102</v>
@@ -2682,13 +2679,13 @@
         <v>102</v>
       </c>
       <c r="P23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q23" t="s">
         <v>102</v>
       </c>
       <c r="R23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S23" t="s">
         <v>102</v>
@@ -2709,7 +2706,7 @@
         <v>102</v>
       </c>
       <c r="Y23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z23" t="s">
         <v>102</v>
@@ -2738,26 +2735,26 @@
         <v>91.21726226806641</v>
       </c>
       <c r="G24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J24" t="s">
         <v>138</v>
       </c>
-      <c r="J24" t="s">
-        <v>139</v>
-      </c>
       <c r="K24" t="s">
+        <v>145</v>
+      </c>
+      <c r="L24" t="s">
+        <v>102</v>
+      </c>
+      <c r="M24" t="s">
         <v>146</v>
       </c>
-      <c r="L24" t="s">
-        <v>102</v>
-      </c>
-      <c r="M24" t="s">
-        <v>147</v>
-      </c>
       <c r="N24" t="s">
         <v>102</v>
       </c>
@@ -2765,13 +2762,13 @@
         <v>102</v>
       </c>
       <c r="P24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q24" t="s">
         <v>102</v>
       </c>
       <c r="R24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S24" t="s">
         <v>102</v>
@@ -2792,7 +2789,7 @@
         <v>102</v>
       </c>
       <c r="Y24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z24" t="s">
         <v>102</v>
@@ -2821,10 +2818,10 @@
         <v>106.0092010498047</v>
       </c>
       <c r="G25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I25" t="s">
         <v>102</v>
@@ -2845,43 +2842,43 @@
         <v>102</v>
       </c>
       <c r="O25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P25" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>102</v>
+      </c>
+      <c r="R25" t="s">
+        <v>102</v>
+      </c>
+      <c r="S25" t="s">
+        <v>102</v>
+      </c>
+      <c r="T25" t="s">
+        <v>102</v>
+      </c>
+      <c r="U25" t="s">
+        <v>102</v>
+      </c>
+      <c r="V25" t="s">
+        <v>102</v>
+      </c>
+      <c r="W25" t="s">
+        <v>147</v>
+      </c>
+      <c r="X25" t="s">
         <v>146</v>
       </c>
-      <c r="Q25" t="s">
-        <v>102</v>
-      </c>
-      <c r="R25" t="s">
-        <v>102</v>
-      </c>
-      <c r="S25" t="s">
-        <v>102</v>
-      </c>
-      <c r="T25" t="s">
-        <v>102</v>
-      </c>
-      <c r="U25" t="s">
-        <v>102</v>
-      </c>
-      <c r="V25" t="s">
-        <v>102</v>
-      </c>
-      <c r="W25" t="s">
-        <v>148</v>
-      </c>
-      <c r="X25" t="s">
-        <v>147</v>
-      </c>
       <c r="Y25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z25" t="s">
         <v>102</v>
       </c>
       <c r="AA25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -2904,25 +2901,25 @@
         <v>94.14483642578125</v>
       </c>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J26" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" t="s">
         <v>146</v>
       </c>
-      <c r="K26" t="s">
-        <v>147</v>
-      </c>
       <c r="L26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N26" t="s">
         <v>102</v>
@@ -2931,7 +2928,7 @@
         <v>102</v>
       </c>
       <c r="P26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q26" t="s">
         <v>102</v>
@@ -2943,7 +2940,7 @@
         <v>102</v>
       </c>
       <c r="T26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U26" t="s">
         <v>102</v>
@@ -2958,7 +2955,7 @@
         <v>102</v>
       </c>
       <c r="Y26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z26" t="s">
         <v>102</v>
@@ -2987,31 +2984,31 @@
         <v>126.3481979370117</v>
       </c>
       <c r="G27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I27" t="s">
         <v>102</v>
       </c>
       <c r="J27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N27" t="s">
         <v>102</v>
       </c>
       <c r="O27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P27" t="s">
         <v>102</v>
@@ -3026,7 +3023,7 @@
         <v>102</v>
       </c>
       <c r="T27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U27" t="s">
         <v>102</v>
@@ -3038,7 +3035,7 @@
         <v>102</v>
       </c>
       <c r="X27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y27" t="s">
         <v>102</v>
@@ -3047,7 +3044,7 @@
         <v>102</v>
       </c>
       <c r="AA27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -3070,40 +3067,40 @@
         <v>96.14791870117188</v>
       </c>
       <c r="G28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H28" t="s">
         <v>102</v>
       </c>
       <c r="I28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K28" t="s">
         <v>102</v>
       </c>
       <c r="L28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O28" t="s">
         <v>102</v>
       </c>
       <c r="P28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q28" t="s">
         <v>102</v>
       </c>
       <c r="R28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S28" t="s">
         <v>102</v>
@@ -3124,10 +3121,10 @@
         <v>102</v>
       </c>
       <c r="Y28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA28" t="s">
         <v>102</v>
@@ -3153,34 +3150,34 @@
         <v>60.24652862548828</v>
       </c>
       <c r="G29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H29" t="s">
         <v>102</v>
       </c>
       <c r="I29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N29" t="s">
         <v>102</v>
       </c>
       <c r="O29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q29" t="s">
         <v>102</v>
@@ -3192,13 +3189,13 @@
         <v>102</v>
       </c>
       <c r="T29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U29" t="s">
         <v>102</v>
       </c>
       <c r="V29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W29" t="s">
         <v>102</v>
@@ -3207,13 +3204,13 @@
         <v>102</v>
       </c>
       <c r="Y29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z29" t="s">
         <v>102</v>
       </c>
       <c r="AA29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -3236,13 +3233,13 @@
         <v>76.42527008056641</v>
       </c>
       <c r="G30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J30" t="s">
         <v>102</v>
@@ -3260,10 +3257,10 @@
         <v>102</v>
       </c>
       <c r="O30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q30" t="s">
         <v>102</v>
@@ -3281,7 +3278,7 @@
         <v>102</v>
       </c>
       <c r="V30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W30" t="s">
         <v>102</v>
@@ -3290,13 +3287,13 @@
         <v>102</v>
       </c>
       <c r="Y30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z30" t="s">
         <v>102</v>
       </c>
       <c r="AA30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -3319,7 +3316,7 @@
         <v>103.5438995361328</v>
       </c>
       <c r="G31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H31" t="s">
         <v>102</v>
@@ -3343,10 +3340,10 @@
         <v>102</v>
       </c>
       <c r="O31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q31" t="s">
         <v>102</v>
@@ -3370,16 +3367,16 @@
         <v>102</v>
       </c>
       <c r="X31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z31" t="s">
         <v>102</v>
       </c>
       <c r="AA31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3402,25 +3399,25 @@
         <v>110.9399032592773</v>
       </c>
       <c r="G32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H32" t="s">
         <v>102</v>
       </c>
       <c r="I32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K32" t="s">
+        <v>137</v>
+      </c>
+      <c r="L32" t="s">
         <v>138</v>
       </c>
-      <c r="L32" t="s">
-        <v>139</v>
-      </c>
       <c r="M32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N32" t="s">
         <v>102</v>
@@ -3429,7 +3426,7 @@
         <v>102</v>
       </c>
       <c r="P32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q32" t="s">
         <v>102</v>
@@ -3438,7 +3435,7 @@
         <v>102</v>
       </c>
       <c r="S32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T32" t="s">
         <v>102</v>
@@ -3456,7 +3453,7 @@
         <v>102</v>
       </c>
       <c r="Y32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z32" t="s">
         <v>102</v>
@@ -3485,7 +3482,7 @@
         <v>138.6748962402344</v>
       </c>
       <c r="G33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H33" t="s">
         <v>102</v>
@@ -3512,7 +3509,7 @@
         <v>102</v>
       </c>
       <c r="P33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q33" t="s">
         <v>102</v>
@@ -3539,7 +3536,7 @@
         <v>102</v>
       </c>
       <c r="Y33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z33" t="s">
         <v>102</v>
@@ -3568,7 +3565,7 @@
         <v>129.4299011230469</v>
       </c>
       <c r="G34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H34" t="s">
         <v>102</v>
@@ -3595,7 +3592,7 @@
         <v>102</v>
       </c>
       <c r="P34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q34" t="s">
         <v>102</v>
@@ -3622,7 +3619,7 @@
         <v>102</v>
       </c>
       <c r="Y34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z34" t="s">
         <v>102</v>
@@ -3648,7 +3645,7 @@
         <v>102</v>
       </c>
       <c r="G35" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H35" t="s">
         <v>102</v>
@@ -3728,7 +3725,7 @@
         <v>102</v>
       </c>
       <c r="G36" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H36" t="s">
         <v>102</v>
@@ -3758,7 +3755,7 @@
         <v>102</v>
       </c>
       <c r="Q36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R36" t="s">
         <v>102</v>
@@ -3808,7 +3805,7 @@
         <v>102</v>
       </c>
       <c r="G37" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H37" t="s">
         <v>102</v>
@@ -3835,10 +3832,10 @@
         <v>102</v>
       </c>
       <c r="P37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R37" t="s">
         <v>102</v>
@@ -3862,7 +3859,7 @@
         <v>102</v>
       </c>
       <c r="Y37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z37" t="s">
         <v>102</v>
@@ -3888,7 +3885,7 @@
         <v>102</v>
       </c>
       <c r="G38" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H38" t="s">
         <v>102</v>
@@ -3915,10 +3912,10 @@
         <v>102</v>
       </c>
       <c r="P38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R38" t="s">
         <v>102</v>
@@ -3942,7 +3939,7 @@
         <v>102</v>
       </c>
       <c r="Y38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z38" t="s">
         <v>102</v>
@@ -3968,7 +3965,7 @@
         <v>102</v>
       </c>
       <c r="G39" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H39" t="s">
         <v>102</v>
@@ -3995,7 +3992,7 @@
         <v>102</v>
       </c>
       <c r="P39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q39" t="s">
         <v>102</v>
@@ -4022,7 +4019,7 @@
         <v>102</v>
       </c>
       <c r="Y39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z39" t="s">
         <v>102</v>
@@ -4048,7 +4045,7 @@
         <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H40" t="s">
         <v>102</v>
@@ -4075,7 +4072,7 @@
         <v>102</v>
       </c>
       <c r="P40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q40" t="s">
         <v>102</v>
@@ -4102,7 +4099,7 @@
         <v>102</v>
       </c>
       <c r="Y40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z40" t="s">
         <v>102</v>
@@ -4128,7 +4125,7 @@
         <v>102</v>
       </c>
       <c r="G41" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H41" t="s">
         <v>102</v>
@@ -4155,7 +4152,7 @@
         <v>102</v>
       </c>
       <c r="P41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q41" t="s">
         <v>102</v>
@@ -4182,7 +4179,7 @@
         <v>102</v>
       </c>
       <c r="Y41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z41" t="s">
         <v>102</v>
@@ -4208,7 +4205,7 @@
         <v>102</v>
       </c>
       <c r="G42" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H42" t="s">
         <v>102</v>
@@ -4235,7 +4232,7 @@
         <v>102</v>
       </c>
       <c r="P42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q42" t="s">
         <v>102</v>
@@ -4262,7 +4259,7 @@
         <v>102</v>
       </c>
       <c r="Y42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z42" t="s">
         <v>102</v>
@@ -4288,7 +4285,7 @@
         <v>102</v>
       </c>
       <c r="G43" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H43" t="s">
         <v>102</v>
@@ -4315,10 +4312,10 @@
         <v>102</v>
       </c>
       <c r="P43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R43" t="s">
         <v>102</v>
@@ -4342,7 +4339,7 @@
         <v>102</v>
       </c>
       <c r="Y43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z43" t="s">
         <v>102</v>
@@ -4368,7 +4365,7 @@
         <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H44" t="s">
         <v>102</v>
@@ -4395,7 +4392,7 @@
         <v>102</v>
       </c>
       <c r="P44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q44" t="s">
         <v>102</v>
@@ -4422,7 +4419,7 @@
         <v>102</v>
       </c>
       <c r="Y44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z44" t="s">
         <v>102</v>
@@ -4448,7 +4445,7 @@
         <v>102</v>
       </c>
       <c r="G45" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H45" t="s">
         <v>102</v>
@@ -4528,67 +4525,67 @@
         <v>102</v>
       </c>
       <c r="G46" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I46" t="s">
         <v>112</v>
       </c>
       <c r="J46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L46" t="s">
+        <v>145</v>
+      </c>
+      <c r="M46" t="s">
+        <v>122</v>
+      </c>
+      <c r="N46" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46" t="s">
+        <v>134</v>
+      </c>
+      <c r="P46" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>102</v>
+      </c>
+      <c r="R46" t="s">
+        <v>102</v>
+      </c>
+      <c r="S46" t="s">
+        <v>134</v>
+      </c>
+      <c r="T46" t="s">
+        <v>102</v>
+      </c>
+      <c r="U46" t="s">
+        <v>102</v>
+      </c>
+      <c r="V46" t="s">
+        <v>102</v>
+      </c>
+      <c r="W46" t="s">
+        <v>102</v>
+      </c>
+      <c r="X46" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y46" t="s">
         <v>146</v>
       </c>
-      <c r="M46" t="s">
-        <v>123</v>
-      </c>
-      <c r="N46" t="s">
-        <v>102</v>
-      </c>
-      <c r="O46" t="s">
-        <v>135</v>
-      </c>
-      <c r="P46" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>102</v>
-      </c>
-      <c r="R46" t="s">
-        <v>102</v>
-      </c>
-      <c r="S46" t="s">
-        <v>135</v>
-      </c>
-      <c r="T46" t="s">
-        <v>102</v>
-      </c>
-      <c r="U46" t="s">
-        <v>102</v>
-      </c>
-      <c r="V46" t="s">
-        <v>102</v>
-      </c>
-      <c r="W46" t="s">
-        <v>102</v>
-      </c>
-      <c r="X46" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>147</v>
-      </c>
       <c r="Z46" t="s">
         <v>102</v>
       </c>
       <c r="AA46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:27">
@@ -4608,7 +4605,7 @@
         <v>102</v>
       </c>
       <c r="G47" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H47" t="s">
         <v>102</v>
@@ -4635,7 +4632,7 @@
         <v>102</v>
       </c>
       <c r="P47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q47" t="s">
         <v>102</v>
@@ -4662,7 +4659,7 @@
         <v>102</v>
       </c>
       <c r="Y47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z47" t="s">
         <v>102</v>
@@ -4688,7 +4685,7 @@
         <v>102</v>
       </c>
       <c r="G48" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H48" t="s">
         <v>102</v>
@@ -4715,7 +4712,7 @@
         <v>102</v>
       </c>
       <c r="P48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q48" t="s">
         <v>102</v>
@@ -4742,7 +4739,7 @@
         <v>102</v>
       </c>
       <c r="Y48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z48" t="s">
         <v>102</v>
@@ -4768,7 +4765,7 @@
         <v>102</v>
       </c>
       <c r="G49" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H49" t="s">
         <v>102</v>
@@ -4848,7 +4845,7 @@
         <v>102</v>
       </c>
       <c r="G50" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H50" t="s">
         <v>102</v>
@@ -4875,7 +4872,7 @@
         <v>102</v>
       </c>
       <c r="P50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q50" t="s">
         <v>102</v>
@@ -4902,7 +4899,7 @@
         <v>102</v>
       </c>
       <c r="Y50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z50" t="s">
         <v>102</v>
@@ -4928,7 +4925,7 @@
         <v>102</v>
       </c>
       <c r="G51" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H51" t="s">
         <v>102</v>
@@ -4955,7 +4952,7 @@
         <v>102</v>
       </c>
       <c r="P51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q51" t="s">
         <v>102</v>
@@ -4982,7 +4979,7 @@
         <v>102</v>
       </c>
       <c r="Y51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z51" t="s">
         <v>102</v>
@@ -5008,7 +5005,7 @@
         <v>102</v>
       </c>
       <c r="G52" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H52" t="s">
         <v>102</v>
@@ -5088,7 +5085,7 @@
         <v>102</v>
       </c>
       <c r="G53" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H53" t="s">
         <v>102</v>
@@ -5115,7 +5112,7 @@
         <v>102</v>
       </c>
       <c r="P53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q53" t="s">
         <v>102</v>
@@ -5142,7 +5139,7 @@
         <v>102</v>
       </c>
       <c r="Y53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z53" t="s">
         <v>102</v>
@@ -5168,53 +5165,53 @@
         <v>102</v>
       </c>
       <c r="G54" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J54" t="s">
+        <v>137</v>
+      </c>
+      <c r="K54" t="s">
+        <v>145</v>
+      </c>
+      <c r="L54" t="s">
+        <v>145</v>
+      </c>
+      <c r="M54" t="s">
+        <v>134</v>
+      </c>
+      <c r="N54" t="s">
+        <v>102</v>
+      </c>
+      <c r="O54" t="s">
+        <v>102</v>
+      </c>
+      <c r="P54" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>102</v>
+      </c>
+      <c r="R54" t="s">
+        <v>102</v>
+      </c>
+      <c r="S54" t="s">
+        <v>134</v>
+      </c>
+      <c r="T54" t="s">
+        <v>102</v>
+      </c>
+      <c r="U54" t="s">
+        <v>102</v>
+      </c>
+      <c r="V54" t="s">
         <v>138</v>
       </c>
-      <c r="K54" t="s">
-        <v>146</v>
-      </c>
-      <c r="L54" t="s">
-        <v>146</v>
-      </c>
-      <c r="M54" t="s">
-        <v>135</v>
-      </c>
-      <c r="N54" t="s">
-        <v>102</v>
-      </c>
-      <c r="O54" t="s">
-        <v>102</v>
-      </c>
-      <c r="P54" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>102</v>
-      </c>
-      <c r="R54" t="s">
-        <v>102</v>
-      </c>
-      <c r="S54" t="s">
-        <v>135</v>
-      </c>
-      <c r="T54" t="s">
-        <v>102</v>
-      </c>
-      <c r="U54" t="s">
-        <v>102</v>
-      </c>
-      <c r="V54" t="s">
-        <v>139</v>
-      </c>
       <c r="W54" t="s">
         <v>102</v>
       </c>
@@ -5222,7 +5219,7 @@
         <v>102</v>
       </c>
       <c r="Y54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z54" t="s">
         <v>102</v>
@@ -5248,7 +5245,7 @@
         <v>102</v>
       </c>
       <c r="G55" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H55" t="s">
         <v>102</v>
@@ -5328,7 +5325,7 @@
         <v>102</v>
       </c>
       <c r="G56" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H56" t="s">
         <v>102</v>
@@ -5408,13 +5405,13 @@
         <v>102</v>
       </c>
       <c r="G57" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H57" t="s">
         <v>102</v>
       </c>
       <c r="I57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J57" t="s">
         <v>102</v>
@@ -5435,7 +5432,7 @@
         <v>102</v>
       </c>
       <c r="P57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q57" t="s">
         <v>102</v>
@@ -5462,7 +5459,7 @@
         <v>102</v>
       </c>
       <c r="Y57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z57" t="s">
         <v>102</v>
@@ -5488,7 +5485,7 @@
         <v>102</v>
       </c>
       <c r="G58" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H58" t="s">
         <v>102</v>
@@ -5515,7 +5512,7 @@
         <v>102</v>
       </c>
       <c r="P58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q58" t="s">
         <v>102</v>
@@ -5542,7 +5539,7 @@
         <v>102</v>
       </c>
       <c r="Y58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z58" t="s">
         <v>102</v>
@@ -5568,7 +5565,7 @@
         <v>102</v>
       </c>
       <c r="G59" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H59" t="s">
         <v>102</v>
@@ -5595,7 +5592,7 @@
         <v>102</v>
       </c>
       <c r="P59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q59" t="s">
         <v>102</v>
@@ -5622,7 +5619,7 @@
         <v>102</v>
       </c>
       <c r="Y59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z59" t="s">
         <v>102</v>
@@ -5648,13 +5645,13 @@
         <v>102</v>
       </c>
       <c r="G60" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H60" t="s">
         <v>102</v>
       </c>
       <c r="I60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J60" t="s">
         <v>102</v>
@@ -5728,32 +5725,32 @@
         <v>102</v>
       </c>
       <c r="G61" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H61" t="s">
         <v>102</v>
       </c>
       <c r="I61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J61" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L61" t="s">
+        <v>145</v>
+      </c>
+      <c r="M61" t="s">
+        <v>102</v>
+      </c>
+      <c r="N61" t="s">
         <v>146</v>
       </c>
-      <c r="M61" t="s">
-        <v>102</v>
-      </c>
-      <c r="N61" t="s">
+      <c r="O61" t="s">
         <v>147</v>
       </c>
-      <c r="O61" t="s">
-        <v>148</v>
-      </c>
       <c r="P61" t="s">
         <v>102</v>
       </c>
@@ -5767,28 +5764,28 @@
         <v>102</v>
       </c>
       <c r="T61" t="s">
+        <v>145</v>
+      </c>
+      <c r="U61" t="s">
+        <v>102</v>
+      </c>
+      <c r="V61" t="s">
+        <v>102</v>
+      </c>
+      <c r="W61" t="s">
+        <v>102</v>
+      </c>
+      <c r="X61" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z61" t="s">
         <v>146</v>
       </c>
-      <c r="U61" t="s">
-        <v>102</v>
-      </c>
-      <c r="V61" t="s">
-        <v>102</v>
-      </c>
-      <c r="W61" t="s">
-        <v>102</v>
-      </c>
-      <c r="X61" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y61" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z61" t="s">
+      <c r="AA61" t="s">
         <v>147</v>
-      </c>
-      <c r="AA61" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:27">
@@ -5808,7 +5805,7 @@
         <v>102</v>
       </c>
       <c r="G62" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H62" t="s">
         <v>102</v>
@@ -5835,7 +5832,7 @@
         <v>102</v>
       </c>
       <c r="P62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q62" t="s">
         <v>102</v>
@@ -5862,7 +5859,7 @@
         <v>102</v>
       </c>
       <c r="Y62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z62" t="s">
         <v>102</v>
@@ -5888,7 +5885,7 @@
         <v>102</v>
       </c>
       <c r="G63" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H63" t="s">
         <v>102</v>
@@ -5968,13 +5965,13 @@
         <v>102</v>
       </c>
       <c r="G64" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J64" t="s">
         <v>102</v>
@@ -5995,22 +5992,22 @@
         <v>102</v>
       </c>
       <c r="P64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q64" t="s">
         <v>102</v>
       </c>
       <c r="R64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S64" t="s">
         <v>102</v>
       </c>
       <c r="T64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V64" t="s">
         <v>102</v>
@@ -6019,10 +6016,10 @@
         <v>102</v>
       </c>
       <c r="X64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Y64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Z64" t="s">
         <v>102</v>
@@ -6048,7 +6045,7 @@
         <v>102</v>
       </c>
       <c r="G65" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H65" t="s">
         <v>102</v>
@@ -6069,13 +6066,13 @@
         <v>102</v>
       </c>
       <c r="N65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O65" t="s">
         <v>102</v>
       </c>
       <c r="P65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q65" t="s">
         <v>102</v>
@@ -6102,10 +6099,10 @@
         <v>102</v>
       </c>
       <c r="Y65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Z65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AA65" t="s">
         <v>102</v>
@@ -6128,13 +6125,13 @@
         <v>102</v>
       </c>
       <c r="G66" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H66" t="s">
         <v>102</v>
       </c>
       <c r="I66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J66" t="s">
         <v>102</v>
@@ -6143,11 +6140,11 @@
         <v>102</v>
       </c>
       <c r="L66" t="s">
+        <v>137</v>
+      </c>
+      <c r="M66" t="s">
         <v>138</v>
       </c>
-      <c r="M66" t="s">
-        <v>139</v>
-      </c>
       <c r="N66" t="s">
         <v>102</v>
       </c>
@@ -6170,7 +6167,7 @@
         <v>102</v>
       </c>
       <c r="U66" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V66" t="s">
         <v>102</v>
@@ -6208,10 +6205,10 @@
         <v>102</v>
       </c>
       <c r="G67" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I67" t="s">
         <v>112</v>
@@ -6232,10 +6229,10 @@
         <v>102</v>
       </c>
       <c r="O67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q67" t="s">
         <v>102</v>
@@ -6253,7 +6250,7 @@
         <v>102</v>
       </c>
       <c r="V67" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W67" t="s">
         <v>102</v>
@@ -6262,13 +6259,13 @@
         <v>102</v>
       </c>
       <c r="Y67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z67" t="s">
         <v>102</v>
       </c>
       <c r="AA67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:27">
@@ -6288,13 +6285,13 @@
         <v>102</v>
       </c>
       <c r="G68" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H68" t="s">
         <v>102</v>
       </c>
       <c r="I68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J68" t="s">
         <v>102</v>
@@ -6368,25 +6365,25 @@
         <v>102</v>
       </c>
       <c r="G69" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H69" t="s">
         <v>102</v>
       </c>
       <c r="I69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J69" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L69" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N69" t="s">
         <v>102</v>
@@ -6410,7 +6407,7 @@
         <v>102</v>
       </c>
       <c r="U69" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V69" t="s">
         <v>102</v>
@@ -6448,19 +6445,19 @@
         <v>102</v>
       </c>
       <c r="G70" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J70" t="s">
         <v>102</v>
       </c>
       <c r="K70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L70" t="s">
         <v>102</v>
@@ -6472,10 +6469,10 @@
         <v>102</v>
       </c>
       <c r="O70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q70" t="s">
         <v>102</v>
@@ -6490,25 +6487,25 @@
         <v>102</v>
       </c>
       <c r="U70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W70" t="s">
         <v>102</v>
       </c>
       <c r="X70" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z70" t="s">
         <v>102</v>
       </c>
       <c r="AA70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:27">
@@ -6528,7 +6525,7 @@
         <v>102</v>
       </c>
       <c r="G71" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="H71" t="s">
         <v>102</v>

</xml_diff>